<commit_message>
Removed Credentials from InputData file
</commit_message>
<xml_diff>
--- a/Amazon/InputData.xlsx
+++ b/Amazon/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7815" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Input Data" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -25,19 +25,13 @@
     <t>input search</t>
   </si>
   <si>
-    <t>$ufiyaN7861</t>
-  </si>
-  <si>
-    <t>sofi.naikwadi786@gmail.com</t>
-  </si>
-  <si>
     <t>OnePlus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,37 +370,31 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>